<commit_message>
Se agrego openxlsx a la lista de paquetes
</commit_message>
<xml_diff>
--- a/paquetes.xlsx
+++ b/paquetes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t xml:space="preserve">PAQUETES</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">corrgram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openxlsx</t>
   </si>
 </sst>
 </file>
@@ -151,6 +154,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -172,6 +176,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,13 +247,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
   </cols>
@@ -451,6 +456,11 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>